<commit_message>
feat: import user with mahasiswa
</commit_message>
<xml_diff>
--- a/public/template/Mahasiswi.xlsx
+++ b/public/template/Mahasiswi.xlsx
@@ -1441,7 +1441,7 @@
     <t>085793578887</t>
   </si>
   <si>
-    <t>someemail@mail.com</t>
+    <t>dimasdzuky99@gmail.com</t>
   </si>
   <si>
     <t>0</t>
@@ -1525,7 +1525,7 @@
     <t>Mobil</t>
   </si>
   <si>
-    <t>budisantoso@mail.com</t>
+    <t>satriayudha262@gmail.com</t>
   </si>
   <si>
     <t>1234567890123450</t>
@@ -1576,7 +1576,7 @@
     <t>Sepeda</t>
   </si>
   <si>
-    <t>sitimaryam@mail.com</t>
+    <t>bathoozar@gmail.com</t>
   </si>
   <si>
     <t>JONATHAN DOE</t>
@@ -1618,7 +1618,7 @@
     <t>Motor</t>
   </si>
   <si>
-    <t>alifahmi@mail.com</t>
+    <t>andikabastian20@gmail.com</t>
   </si>
   <si>
     <t>AMIR AYAH</t>
@@ -1654,7 +1654,7 @@
     <t>Kenanga</t>
   </si>
   <si>
-    <t>rinap@mail.com</t>
+    <t>rinap@gmail.com</t>
   </si>
   <si>
     <t>BAHRI AYAH</t>
@@ -1690,7 +1690,7 @@
     <t>Bunga</t>
   </si>
   <si>
-    <t>andiw@mail.com</t>
+    <t>andiw@gmail.com</t>
   </si>
   <si>
     <t>1234567890123460</t>
@@ -1729,7 +1729,7 @@
     <t>Mawar</t>
   </si>
   <si>
-    <t>dina@mail.com</t>
+    <t>dina@gmail.com</t>
   </si>
   <si>
     <t>SAMSUL AYAH</t>
@@ -1765,7 +1765,7 @@
     <t>Jati</t>
   </si>
   <si>
-    <t>hendra@mail.com</t>
+    <t>hendra@gmail.com</t>
   </si>
   <si>
     <t>JANI AYAH</t>
@@ -1795,7 +1795,7 @@
     <t>123456123456130</t>
   </si>
   <si>
-    <t>sandraputri@mail.com</t>
+    <t>sandraputri@gmail.com</t>
   </si>
   <si>
     <t>AMAN AYAH</t>
@@ -1868,6 +1868,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <name val="Consolas"/>
       <charset val="134"/>
@@ -1881,22 +1897,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2400,10 +2400,10 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
@@ -2530,7 +2530,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2570,6 +2570,12 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2579,16 +2585,16 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -3132,8 +3138,8 @@
   <sheetPr/>
   <dimension ref="A1:BB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG2" workbookViewId="0">
-      <selection activeCell="AG10" sqref="AG10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3310,22 +3316,22 @@
       <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="13" t="s">
+      <c r="AU1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="14" t="s">
+      <c r="AV1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="14" t="s">
+      <c r="AW1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="AX1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="14" t="s">
+      <c r="AY1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="14" t="s">
+      <c r="AZ1" s="16" t="s">
         <v>51</v>
       </c>
       <c r="BA1" s="6" t="s">
@@ -3408,7 +3414,7 @@
       <c r="X2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="Y2" s="20" t="s">
+      <c r="Y2" s="22" t="s">
         <v>71</v>
       </c>
       <c r="Z2" s="12" t="s">
@@ -3454,43 +3460,43 @@
       <c r="AN2" s="2">
         <v>13</v>
       </c>
-      <c r="AO2" s="15" t="s">
+      <c r="AO2" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="AP2" s="15" t="s">
+      <c r="AP2" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="AQ2" s="15" t="s">
+      <c r="AQ2" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="AR2" s="15" t="s">
+      <c r="AR2" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="AS2" s="15" t="s">
+      <c r="AS2" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AT2" s="16" t="s">
+      <c r="AT2" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="AU2" s="17" t="s">
+      <c r="AU2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="AV2" s="18" t="s">
+      <c r="AV2" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AW2" s="18" t="s">
+      <c r="AW2" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AX2" s="18" t="s">
+      <c r="AX2" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="AY2" s="16" t="s">
+      <c r="AY2" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="AZ2" s="15" t="s">
+      <c r="AZ2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="BA2" s="15">
+      <c r="BA2" s="17">
         <v>1</v>
       </c>
       <c r="BB2" s="2">
@@ -3513,7 +3519,7 @@
       <c r="E3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="23" t="s">
         <v>93</v>
       </c>
       <c r="G3" s="3">
@@ -3525,7 +3531,7 @@
       <c r="I3" s="3">
         <v>5</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="23" t="s">
         <v>94</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -3573,14 +3579,14 @@
       <c r="Y3" s="3">
         <v>81234567890</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="Z3" s="13" t="s">
         <v>100</v>
       </c>
       <c r="AA3" s="3">
         <v>1</v>
       </c>
       <c r="AB3" s="3"/>
-      <c r="AC3" s="21" t="s">
+      <c r="AC3" s="23" t="s">
         <v>101</v>
       </c>
       <c r="AD3" s="3" t="s">
@@ -3598,7 +3604,7 @@
       <c r="AH3" s="3">
         <v>11</v>
       </c>
-      <c r="AI3" s="21" t="s">
+      <c r="AI3" s="23" t="s">
         <v>101</v>
       </c>
       <c r="AJ3" s="3" t="s">
@@ -3628,25 +3634,25 @@
       <c r="AR3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AS3" s="15" t="s">
+      <c r="AS3" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AT3" s="16" t="s">
+      <c r="AT3" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="AU3" s="19" t="s">
+      <c r="AU3" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="AV3" s="19">
+      <c r="AV3" s="21">
         <v>21</v>
       </c>
-      <c r="AW3" s="19">
+      <c r="AW3" s="21">
         <v>2001</v>
       </c>
-      <c r="AX3" s="19" t="s">
+      <c r="AX3" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="AY3" s="16" t="s">
+      <c r="AY3" s="18" t="s">
         <v>84</v>
       </c>
       <c r="AZ3" s="3" t="s">
@@ -3675,7 +3681,7 @@
       <c r="E4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="23" t="s">
         <v>112</v>
       </c>
       <c r="G4" s="3">
@@ -3687,7 +3693,7 @@
       <c r="I4" s="3">
         <v>1</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="23" t="s">
         <v>113</v>
       </c>
       <c r="K4" s="3" t="s">
@@ -3735,14 +3741,14 @@
       <c r="Y4" s="3">
         <v>82345678901</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="Z4" s="14" t="s">
         <v>117</v>
       </c>
       <c r="AA4" s="3">
         <v>0</v>
       </c>
       <c r="AB4" s="3"/>
-      <c r="AC4" s="21" t="s">
+      <c r="AC4" s="23" t="s">
         <v>101</v>
       </c>
       <c r="AD4" s="3" t="s">
@@ -3760,7 +3766,7 @@
       <c r="AH4" s="3">
         <v>12</v>
       </c>
-      <c r="AI4" s="21" t="s">
+      <c r="AI4" s="23" t="s">
         <v>101</v>
       </c>
       <c r="AJ4" s="3" t="s">
@@ -3790,32 +3796,32 @@
       <c r="AR4" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AS4" s="15" t="s">
+      <c r="AS4" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AT4" s="16" t="s">
+      <c r="AT4" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="AU4" s="19" t="s">
+      <c r="AU4" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="AV4" s="19">
+      <c r="AV4" s="21">
         <v>21</v>
       </c>
-      <c r="AW4" s="19">
+      <c r="AW4" s="21">
         <v>2002</v>
       </c>
-      <c r="AX4" s="19" t="s">
+      <c r="AX4" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="AY4" s="16" t="s">
+      <c r="AY4" s="18" t="s">
         <v>121</v>
       </c>
       <c r="AZ4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="BA4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BB4" s="3">
         <v>6500000</v>
@@ -3837,7 +3843,7 @@
       <c r="E5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="23" t="s">
         <v>126</v>
       </c>
       <c r="G5" s="3">
@@ -3849,7 +3855,7 @@
       <c r="I5" s="3">
         <v>4</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="23" t="s">
         <v>127</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -3897,14 +3903,14 @@
       <c r="Y5" s="3">
         <v>83456789012</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="Z5" s="14" t="s">
         <v>131</v>
       </c>
       <c r="AA5" s="3">
         <v>1</v>
       </c>
       <c r="AB5" s="3"/>
-      <c r="AC5" s="21" t="s">
+      <c r="AC5" s="23" t="s">
         <v>101</v>
       </c>
       <c r="AD5" s="3" t="s">
@@ -3922,7 +3928,7 @@
       <c r="AH5" s="3">
         <v>14</v>
       </c>
-      <c r="AI5" s="21" t="s">
+      <c r="AI5" s="23" t="s">
         <v>101</v>
       </c>
       <c r="AJ5" s="3" t="s">
@@ -3952,32 +3958,32 @@
       <c r="AR5" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AS5" s="15" t="s">
+      <c r="AS5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AT5" s="16" t="s">
+      <c r="AT5" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="AU5" s="19" t="s">
+      <c r="AU5" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="AV5" s="19">
+      <c r="AV5" s="21">
         <v>21</v>
       </c>
-      <c r="AW5" s="19">
+      <c r="AW5" s="21">
         <v>2003</v>
       </c>
-      <c r="AX5" s="19" t="s">
+      <c r="AX5" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="AY5" s="16" t="s">
+      <c r="AY5" s="18" t="s">
         <v>134</v>
       </c>
       <c r="AZ5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="BA5" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BB5" s="3">
         <v>7000000</v>
@@ -3999,7 +4005,7 @@
       <c r="E6" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="23" t="s">
         <v>139</v>
       </c>
       <c r="G6" s="3">
@@ -4011,7 +4017,7 @@
       <c r="I6" s="3">
         <v>5</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="23" t="s">
         <v>140</v>
       </c>
       <c r="K6" s="3" t="s">
@@ -4059,14 +4065,14 @@
       <c r="Y6" s="3">
         <v>84567890123</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="Z6" s="13" t="s">
         <v>143</v>
       </c>
       <c r="AA6" s="3">
         <v>0</v>
       </c>
       <c r="AB6" s="3"/>
-      <c r="AC6" s="21" t="s">
+      <c r="AC6" s="23" t="s">
         <v>101</v>
       </c>
       <c r="AD6" s="3" t="s">
@@ -4084,7 +4090,7 @@
       <c r="AH6" s="3">
         <v>12</v>
       </c>
-      <c r="AI6" s="21" t="s">
+      <c r="AI6" s="23" t="s">
         <v>101</v>
       </c>
       <c r="AJ6" s="3" t="s">
@@ -4114,32 +4120,32 @@
       <c r="AR6" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AS6" s="15" t="s">
+      <c r="AS6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AT6" s="16" t="s">
+      <c r="AT6" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="AU6" s="19" t="s">
+      <c r="AU6" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="AV6" s="19">
+      <c r="AV6" s="21">
         <v>21</v>
       </c>
-      <c r="AW6" s="19">
+      <c r="AW6" s="21">
         <v>2004</v>
       </c>
-      <c r="AX6" s="19" t="s">
+      <c r="AX6" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="AY6" s="16" t="s">
+      <c r="AY6" s="18" t="s">
         <v>121</v>
       </c>
       <c r="AZ6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="BA6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BB6" s="3">
         <v>5500000</v>
@@ -4161,7 +4167,7 @@
       <c r="E7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="23" t="s">
         <v>151</v>
       </c>
       <c r="G7" s="3">
@@ -4173,7 +4179,7 @@
       <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="23" t="s">
         <v>152</v>
       </c>
       <c r="K7" s="3" t="s">
@@ -4221,14 +4227,14 @@
       <c r="Y7" s="3">
         <v>85678901234</v>
       </c>
-      <c r="Z7" s="3" t="s">
+      <c r="Z7" s="13" t="s">
         <v>155</v>
       </c>
       <c r="AA7" s="3">
         <v>1</v>
       </c>
       <c r="AB7" s="3"/>
-      <c r="AC7" s="21" t="s">
+      <c r="AC7" s="23" t="s">
         <v>156</v>
       </c>
       <c r="AD7" s="3" t="s">
@@ -4246,7 +4252,7 @@
       <c r="AH7" s="3">
         <v>12</v>
       </c>
-      <c r="AI7" s="21" t="s">
+      <c r="AI7" s="23" t="s">
         <v>156</v>
       </c>
       <c r="AJ7" s="3" t="s">
@@ -4279,22 +4285,22 @@
       <c r="AS7" s="3">
         <v>12</v>
       </c>
-      <c r="AT7" s="16" t="s">
+      <c r="AT7" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="AU7" s="19" t="s">
+      <c r="AU7" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="AV7" s="19">
+      <c r="AV7" s="21">
         <v>21</v>
       </c>
-      <c r="AW7" s="19">
+      <c r="AW7" s="21">
         <v>2005</v>
       </c>
-      <c r="AX7" s="19" t="s">
+      <c r="AX7" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="AY7" s="16" t="s">
+      <c r="AY7" s="18" t="s">
         <v>84</v>
       </c>
       <c r="AZ7" s="3" t="s">
@@ -4323,7 +4329,7 @@
       <c r="E8" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="23" t="s">
         <v>164</v>
       </c>
       <c r="G8" s="3">
@@ -4335,7 +4341,7 @@
       <c r="I8" s="3">
         <v>5</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="23" t="s">
         <v>165</v>
       </c>
       <c r="K8" s="3" t="s">
@@ -4383,14 +4389,14 @@
       <c r="Y8" s="3">
         <v>86789012345</v>
       </c>
-      <c r="Z8" s="3" t="s">
+      <c r="Z8" s="13" t="s">
         <v>168</v>
       </c>
       <c r="AA8" s="3">
         <v>1</v>
       </c>
       <c r="AB8" s="3"/>
-      <c r="AC8" s="21" t="s">
+      <c r="AC8" s="23" t="s">
         <v>156</v>
       </c>
       <c r="AD8" s="3" t="s">
@@ -4408,7 +4414,7 @@
       <c r="AH8" s="3">
         <v>12</v>
       </c>
-      <c r="AI8" s="21" t="s">
+      <c r="AI8" s="23" t="s">
         <v>156</v>
       </c>
       <c r="AJ8" s="3" t="s">
@@ -4441,22 +4447,22 @@
       <c r="AS8" s="3">
         <v>13</v>
       </c>
-      <c r="AT8" s="16" t="s">
+      <c r="AT8" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="AU8" s="19" t="s">
+      <c r="AU8" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="AV8" s="19">
+      <c r="AV8" s="21">
         <v>21</v>
       </c>
-      <c r="AW8" s="19">
+      <c r="AW8" s="21">
         <v>2006</v>
       </c>
-      <c r="AX8" s="19" t="s">
+      <c r="AX8" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="AY8" s="16" t="s">
+      <c r="AY8" s="18" t="s">
         <v>134</v>
       </c>
       <c r="AZ8" s="3" t="s">
@@ -4485,7 +4491,7 @@
       <c r="E9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="23" t="s">
         <v>176</v>
       </c>
       <c r="G9" s="3">
@@ -4497,7 +4503,7 @@
       <c r="I9" s="3">
         <v>1</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="23" t="s">
         <v>177</v>
       </c>
       <c r="K9" s="3" t="s">
@@ -4545,14 +4551,14 @@
       <c r="Y9" s="3">
         <v>87890123456</v>
       </c>
-      <c r="Z9" s="3" t="s">
+      <c r="Z9" s="13" t="s">
         <v>180</v>
       </c>
       <c r="AA9" s="3">
         <v>0</v>
       </c>
       <c r="AB9" s="3"/>
-      <c r="AC9" s="21" t="s">
+      <c r="AC9" s="23" t="s">
         <v>156</v>
       </c>
       <c r="AD9" s="3" t="s">
@@ -4570,7 +4576,7 @@
       <c r="AH9" s="3">
         <v>11</v>
       </c>
-      <c r="AI9" s="21" t="s">
+      <c r="AI9" s="23" t="s">
         <v>156</v>
       </c>
       <c r="AJ9" s="3" t="s">
@@ -4603,22 +4609,22 @@
       <c r="AS9" s="3">
         <v>12</v>
       </c>
-      <c r="AT9" s="16" t="s">
+      <c r="AT9" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="AU9" s="19" t="s">
+      <c r="AU9" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="AV9" s="19">
+      <c r="AV9" s="21">
         <v>21</v>
       </c>
-      <c r="AW9" s="19">
+      <c r="AW9" s="21">
         <v>2007</v>
       </c>
-      <c r="AX9" s="19" t="s">
+      <c r="AX9" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="AY9" s="16" t="s">
+      <c r="AY9" s="18" t="s">
         <v>184</v>
       </c>
       <c r="AZ9" s="3" t="s">
@@ -4647,7 +4653,7 @@
       <c r="E10" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="23" t="s">
         <v>188</v>
       </c>
       <c r="G10" s="3">
@@ -4659,7 +4665,7 @@
       <c r="I10" s="3">
         <v>4</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="23" t="s">
         <v>189</v>
       </c>
       <c r="K10" s="3" t="s">
@@ -4707,14 +4713,14 @@
       <c r="Y10" s="3">
         <v>88901234567</v>
       </c>
-      <c r="Z10" s="3" t="s">
+      <c r="Z10" s="13" t="s">
         <v>190</v>
       </c>
       <c r="AA10" s="3">
         <v>1</v>
       </c>
       <c r="AB10" s="3"/>
-      <c r="AC10" s="21" t="s">
+      <c r="AC10" s="23" t="s">
         <v>156</v>
       </c>
       <c r="AD10" s="3" t="s">
@@ -4732,7 +4738,7 @@
       <c r="AH10" s="3">
         <v>13</v>
       </c>
-      <c r="AI10" s="21" t="s">
+      <c r="AI10" s="23" t="s">
         <v>156</v>
       </c>
       <c r="AJ10" s="3" t="s">
@@ -4765,29 +4771,29 @@
       <c r="AS10" s="3">
         <v>12</v>
       </c>
-      <c r="AT10" s="16" t="s">
+      <c r="AT10" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="AU10" s="19" t="s">
+      <c r="AU10" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="AV10" s="19">
+      <c r="AV10" s="21">
         <v>21</v>
       </c>
-      <c r="AW10" s="19">
+      <c r="AW10" s="21">
         <v>2008</v>
       </c>
-      <c r="AX10" s="19" t="s">
+      <c r="AX10" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="AY10" s="16" t="s">
+      <c r="AY10" s="18" t="s">
         <v>184</v>
       </c>
       <c r="AZ10" s="3" t="s">
         <v>108</v>
       </c>
       <c r="BA10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BB10" s="3">
         <v>7000000</v>
@@ -4839,19 +4845,27 @@
       <c r="AQ11" s="3"/>
       <c r="AR11" s="3"/>
       <c r="AS11" s="3"/>
-      <c r="AT11" s="16"/>
-      <c r="AU11" s="19"/>
-      <c r="AV11" s="19"/>
-      <c r="AW11" s="19"/>
-      <c r="AX11" s="19"/>
-      <c r="AY11" s="16"/>
+      <c r="AT11" s="18"/>
+      <c r="AU11" s="21"/>
+      <c r="AV11" s="21"/>
+      <c r="AW11" s="21"/>
+      <c r="AX11" s="21"/>
+      <c r="AY11" s="18"/>
       <c r="AZ11" s="3"/>
       <c r="BA11" s="3"/>
       <c r="BB11" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Z2" r:id="rId3" display="someemail@mail.com" tooltip="mailto:someemail@mail.com"/>
+    <hyperlink ref="Z2" r:id="rId3" display="dimasdzuky99@gmail.com" tooltip="mailto:dimasdzuky99@gmail.com"/>
+    <hyperlink ref="Z3" r:id="rId4" display="satriayudha262@gmail.com"/>
+    <hyperlink ref="Z4" r:id="rId5" display="bathoozar@gmail.com" tooltip="mailto:bathoozar@gmail.com"/>
+    <hyperlink ref="Z5" r:id="rId6" display="andikabastian20@gmail.com" tooltip="mailto:andikabastian20@gmail.com"/>
+    <hyperlink ref="Z6" r:id="rId7" display="rinap@gmail.com"/>
+    <hyperlink ref="Z7" r:id="rId8" display="andiw@gmail.com"/>
+    <hyperlink ref="Z8" r:id="rId9" display="dina@gmail.com"/>
+    <hyperlink ref="Z9" r:id="rId10" display="hendra@gmail.com"/>
+    <hyperlink ref="Z10" r:id="rId11" display="sandraputri@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>